<commit_message>
Se egrego paso extra si llega a fallar la desactivacion del plugin
</commit_message>
<xml_diff>
--- a/cambios/RFCXXXX/Plan de liberaciones v9.0 RFC----..xlsx
+++ b/cambios/RFCXXXX/Plan de liberaciones v9.0 RFC----..xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgonzalo\Documents\cambios\Cambios\Carga de Tablas y conteos - Ciclo de Inversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\githubppm\PPM\cambios\RFCXXXX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E682355-40E8-4D50-B5CF-1BEFF0195251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55AB9A5-B19C-4257-9FFB-15AC1C0EB4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="3936" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Trabajo" sheetId="29" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Hoja1" sheetId="30" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plan de Trabajo'!$A$1:$U$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plan de Trabajo'!$A$1:$U$50</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Plan de Trabajo'!$1:$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="162">
   <si>
     <t>Nombre</t>
   </si>
@@ -402,9 +402,6 @@
     <t>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</t>
   </si>
   <si>
-    <t>Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</t>
-  </si>
-  <si>
     <t>SUBGERENCIA DE INFRAESTRUCTURA DE TI</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
 Para facilitar la visualización de datos actualizados y mejorar la eficiencia en la gestión de contenido del portal.
 ¿Por qué?
 Porque actualmente este proceso es manual y propenso a errores. Automatizarlo permitirá ahorrar tiempo, reducir errores de captura y mantener la información siempre actualizada.</t>
-  </si>
-  <si>
-    <t>015/07/2025</t>
   </si>
   <si>
     <t>Despliegue de tablas de proyectos y conteo de redes de alianza de forma automatizada en las paginas de clicos de inversion en el del Portal Proyectos México (BNOPNEWPPM-A)</t>
@@ -856,8 +850,14 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Revertir cambios en la pagina de ciclos de inversión que se edito:
+    <t>Visualización de datos actualizados de las tablas de proyectos y conteos de redes de alianza</t>
+  </si>
+  <si>
+    <t>En las secciones de proyectos se deben desplegar las tablas y en la seccion de redes de alianza los conteos en sus respectivos idiomas para ambos casos</t>
+  </si>
+  <si>
+    <r>
+      <t>Revertir cambios en las paginas de ciclos de inversión que se editaron:
    -</t>
     </r>
     <r>
@@ -885,19 +885,66 @@
     </r>
   </si>
   <si>
-    <t>Editar una de la paginas de los ciclos de inversion y  colocar los shortcodes correspondientes a la seccion de proyectos y redes de alianza de acuerdo al idioma.
+    <r>
+      <t xml:space="preserve">Editar las paginas de los ciclos de inversion y  colocar los shortcodes correspondientes a la seccion de proyectos y redes de alianza de acuerdo al idioma.
 Español:
-[tabla_sector_idioma idioma=”es”]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[tabla_sector_idioma idioma=”es”]
 [conteo_procura_auto idioma=”es”]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 Ingles
-[tabla_sector_idioma idioma=”en”]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[tabla_sector_idioma idioma=”en”]
 [conteo_procura_auto idioma=”en”]</t>
-  </si>
-  <si>
-    <t>Visualización de datos actualizados de las tablas de proyectos y conteos de redes de alianza</t>
-  </si>
-  <si>
-    <t>En las secciones de proyectos se deben desplegar las tablas y en la seccion de redes de alianza los conteos en sus respectivos idiomas para ambos casos</t>
+    </r>
+  </si>
+  <si>
+    <t>Jesus Gonzalez, Gabriel Flores  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</t>
+  </si>
+  <si>
+    <t>Leonardo Vera, Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</t>
+  </si>
+  <si>
+    <r>
+      <t>En caso de que al desactivar el plugin marque error, se debera ejecutar el siguiente comando:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> rm -rf /app/apache2/htdocs/wp-content/plugins/tabla-sector-conteo</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1331,6 +1378,53 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1343,207 +1437,160 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1970,10 +2017,10 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:T39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,145 +2050,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="66" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="69" t="s">
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="69"/>
-      <c r="S1" s="70" t="s">
+      <c r="R1" s="73"/>
+      <c r="S1" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="70"/>
+      <c r="T1" s="74"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
     </row>
     <row r="4" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="74" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="R4" s="75"/>
-      <c r="S4" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="T4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="83">
+        <v>45866</v>
+      </c>
+      <c r="T4" s="84"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="80"/>
-      <c r="T5" s="81"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="86"/>
     </row>
     <row r="6" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="71" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="66" t="s">
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
       <c r="U6" s="5"/>
     </row>
     <row r="7" spans="1:21" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2168,457 +2215,457 @@
     </row>
     <row r="8" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="53"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
       <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="82" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="82"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="87"/>
       <c r="G9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="54" t="s">
+      <c r="H9" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="55"/>
-      <c r="J9" s="58" t="s">
+      <c r="I9" s="90"/>
+      <c r="J9" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="59"/>
-      <c r="L9" s="63" t="s">
+      <c r="K9" s="92"/>
+      <c r="L9" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="64"/>
-      <c r="N9" s="65"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="98"/>
       <c r="O9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="P9" s="60" t="s">
+      <c r="P9" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="61"/>
-      <c r="S9" s="61"/>
-      <c r="T9" s="62"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="94"/>
+      <c r="S9" s="94"/>
+      <c r="T9" s="95"/>
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="72"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="72"/>
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="72"/>
+      <c r="R12" s="72"/>
+      <c r="S12" s="72"/>
+      <c r="T12" s="72"/>
       <c r="U12" s="5"/>
     </row>
     <row r="13" spans="1:21" ht="88.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="72"/>
+      <c r="R13" s="72"/>
+      <c r="S13" s="72"/>
+      <c r="T13" s="72"/>
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57" t="s">
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="72"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="72"/>
+      <c r="S14" s="72"/>
+      <c r="T14" s="72"/>
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57" t="s">
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
+      <c r="S15" s="72"/>
+      <c r="T15" s="72"/>
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57" t="s">
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="72"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="72"/>
+      <c r="T16" s="72"/>
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57" t="s">
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="57"/>
-      <c r="P17" s="57"/>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="57"/>
-      <c r="S17" s="57"/>
-      <c r="T17" s="57"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="72"/>
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57" t="s">
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="57"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="57"/>
-      <c r="R18" s="57"/>
-      <c r="S18" s="57"/>
-      <c r="T18" s="57"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="72"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="72"/>
+      <c r="T18" s="72"/>
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:22" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="57" t="s">
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="57"/>
-      <c r="R19" s="57"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="57"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
       <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:22" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
-      <c r="P20" s="52"/>
-      <c r="Q20" s="52"/>
-      <c r="R20" s="52"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="99"/>
+      <c r="M20" s="99"/>
+      <c r="N20" s="99"/>
+      <c r="O20" s="99"/>
+      <c r="P20" s="99"/>
+      <c r="Q20" s="99"/>
+      <c r="R20" s="99"/>
+      <c r="S20" s="99"/>
+      <c r="T20" s="99"/>
     </row>
     <row r="21" spans="1:22" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
       <c r="U21" s="9"/>
     </row>
     <row r="22" spans="1:22" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="53"/>
-      <c r="T22" s="53"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
       <c r="U22" s="9"/>
     </row>
     <row r="23" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47" t="s">
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="L23" s="47" t="s">
+      <c r="L23" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47" t="s">
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="Q23" s="47"/>
-      <c r="R23" s="47"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="47"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
     </row>
     <row r="24" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47" t="s">
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="Q24" s="47"/>
+      <c r="Q24" s="46"/>
       <c r="R24" s="11" t="s">
         <v>4</v>
       </c>
@@ -2634,35 +2681,35 @@
       <c r="B25" s="13">
         <v>1</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
       <c r="K25" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="51" t="s">
+      <c r="L25" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="45">
-        <v>45854</v>
-      </c>
-      <c r="Q25" s="46"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="41">
+        <v>45875</v>
+      </c>
+      <c r="Q25" s="42"/>
       <c r="R25" s="14">
-        <v>0.48055555555555557</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="S25" s="14">
         <f>R25+T25</f>
-        <v>0.4826388888888889</v>
+        <v>0.46041666666666664</v>
       </c>
       <c r="T25" s="25">
         <v>2.0833333333333333E-3</v>
@@ -2675,38 +2722,38 @@
       <c r="B26" s="13">
         <v>2</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
+      <c r="C26" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="56"/>
       <c r="K26" s="13">
         <v>1</v>
       </c>
-      <c r="L26" s="51" t="str">
+      <c r="L26" s="57" t="str">
         <f>L25</f>
         <v>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</v>
       </c>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="45">
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="41">
         <f t="shared" ref="P26" si="0">P25</f>
-        <v>45854</v>
-      </c>
-      <c r="Q26" s="46"/>
+        <v>45875</v>
+      </c>
+      <c r="Q26" s="42"/>
       <c r="R26" s="14">
         <f t="shared" ref="R26" si="1">S25</f>
-        <v>0.4826388888888889</v>
+        <v>0.46041666666666664</v>
       </c>
       <c r="S26" s="14">
         <f t="shared" ref="S26" si="2">R26+T26</f>
-        <v>0.48541666666666666</v>
+        <v>0.46319444444444441</v>
       </c>
       <c r="T26" s="25">
         <v>2.7777777777777779E-3</v>
@@ -2716,27 +2763,27 @@
     </row>
     <row r="27" spans="1:22" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
       <c r="U27" s="9"/>
     </row>
     <row r="28" spans="1:22" s="9" customFormat="1" ht="98.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -2744,37 +2791,37 @@
       <c r="B28" s="13">
         <v>3</v>
       </c>
-      <c r="C28" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="C28" s="100" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
       <c r="K28" s="13">
         <v>2</v>
       </c>
-      <c r="L28" s="51" t="str">
+      <c r="L28" s="57" t="str">
         <f>L26</f>
         <v>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</v>
       </c>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="45" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q28" s="46"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="41">
+        <f>P26</f>
+        <v>45875</v>
+      </c>
+      <c r="Q28" s="42"/>
       <c r="R28" s="14">
-        <v>0.5</v>
+        <v>0.46319444444444446</v>
       </c>
       <c r="S28" s="14">
         <f>R28+T28</f>
-        <v>0.50347222222222221</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="T28" s="25">
         <v>3.472222222222222E-3</v>
@@ -2787,38 +2834,38 @@
       <c r="B29" s="13">
         <v>4</v>
       </c>
-      <c r="C29" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="43"/>
+      <c r="C29" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
       <c r="K29" s="13">
         <v>3</v>
       </c>
-      <c r="L29" s="51" t="str">
+      <c r="L29" s="57" t="str">
         <f>L28</f>
         <v>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</v>
       </c>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="45" t="e">
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="41">
         <f>P28</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q29" s="46"/>
+        <v>45875</v>
+      </c>
+      <c r="Q29" s="42"/>
       <c r="R29" s="14">
         <f t="shared" ref="R29" si="3">S28</f>
-        <v>0.50347222222222221</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="S29" s="14">
         <f t="shared" ref="S29" si="4">R29+T29</f>
-        <v>0.50624999999999998</v>
+        <v>0.46944444444444444</v>
       </c>
       <c r="T29" s="25">
         <v>2.7777777777777779E-3</v>
@@ -2831,40 +2878,40 @@
       <c r="B30" s="13">
         <v>5</v>
       </c>
-      <c r="C30" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
+      <c r="C30" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="56"/>
       <c r="K30" s="13">
         <v>4</v>
       </c>
-      <c r="L30" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="45" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S30" s="14" t="e">
-        <f t="shared" ref="S30" si="5">R30+T30</f>
-        <v>#REF!</v>
+      <c r="L30" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="41">
+        <f>P28</f>
+        <v>45875</v>
+      </c>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="14">
+        <f>S29</f>
+        <v>0.46944444444444444</v>
+      </c>
+      <c r="S30" s="14">
+        <f>R30+T30</f>
+        <v>0.47222222222222221</v>
       </c>
       <c r="T30" s="25">
-        <v>1.3194444444444444E-2</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="U30" s="15"/>
       <c r="V30" s="16"/>
@@ -2874,40 +2921,40 @@
       <c r="B31" s="35">
         <v>6</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="56"/>
       <c r="K31" s="35">
         <v>4</v>
       </c>
-      <c r="L31" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="45" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="36" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S31" s="36" t="e">
-        <f t="shared" ref="S31" si="6">R31+T31</f>
-        <v>#REF!</v>
+      <c r="L31" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="41">
+        <f>P30</f>
+        <v>45875</v>
+      </c>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="36">
+        <f>S30</f>
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="S31" s="36">
+        <f t="shared" ref="S31" si="5">R31+T31</f>
+        <v>0.5</v>
       </c>
       <c r="T31" s="40">
-        <v>1.3194444444444444E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="U31" s="37"/>
       <c r="V31" s="38"/>
@@ -2917,38 +2964,38 @@
       <c r="B32" s="13">
         <v>7</v>
       </c>
-      <c r="C32" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="43"/>
+      <c r="C32" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="56"/>
       <c r="K32" s="13">
         <v>5</v>
       </c>
-      <c r="L32" s="51" t="str">
-        <f>L30</f>
-        <v>Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
-      </c>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="45" t="e">
+      <c r="L32" s="57" t="str">
+        <f>L31</f>
+        <v>Leonardo Vera, Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
+      </c>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="41">
         <f>P30</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="14" t="e">
-        <f>S30</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S32" s="14" t="e">
-        <f t="shared" ref="S32" si="7">R32+T32</f>
-        <v>#REF!</v>
+        <v>45875</v>
+      </c>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="14">
+        <f>S31</f>
+        <v>0.5</v>
+      </c>
+      <c r="S32" s="14">
+        <f t="shared" ref="S32" si="6">R32+T32</f>
+        <v>0.51388888888888884</v>
       </c>
       <c r="T32" s="25">
         <v>1.3888888888888888E-2</v>
@@ -2982,208 +3029,208 @@
     </row>
     <row r="34" spans="1:22" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="68"/>
-      <c r="R34" s="68"/>
-      <c r="S34" s="68"/>
-      <c r="T34" s="68"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="101"/>
+      <c r="N34" s="101"/>
+      <c r="O34" s="101"/>
+      <c r="P34" s="101"/>
+      <c r="Q34" s="101"/>
+      <c r="R34" s="101"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
       <c r="U34" s="17"/>
     </row>
     <row r="35" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="53"/>
-      <c r="T35" s="53"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
     </row>
     <row r="36" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
-      <c r="S36" s="57"/>
-      <c r="T36" s="57"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="72"/>
+      <c r="N36" s="72"/>
+      <c r="O36" s="72"/>
+      <c r="P36" s="72"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="72"/>
+      <c r="S36" s="72"/>
+      <c r="T36" s="72"/>
       <c r="U36" s="5"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="57"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="57"/>
-      <c r="P37" s="57"/>
-      <c r="Q37" s="57"/>
-      <c r="R37" s="57"/>
-      <c r="S37" s="57"/>
-      <c r="T37" s="57"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
+      <c r="O37" s="72"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="72"/>
+      <c r="R37" s="72"/>
+      <c r="S37" s="72"/>
+      <c r="T37" s="72"/>
       <c r="U37" s="5"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="57"/>
-      <c r="S38" s="57"/>
-      <c r="T38" s="57"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="72"/>
+      <c r="N38" s="72"/>
+      <c r="O38" s="72"/>
+      <c r="P38" s="72"/>
+      <c r="Q38" s="72"/>
+      <c r="R38" s="72"/>
+      <c r="S38" s="72"/>
+      <c r="T38" s="72"/>
       <c r="U38" s="5"/>
     </row>
     <row r="39" spans="1:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="53"/>
-      <c r="T39" s="53"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="47"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="47"/>
+      <c r="P39" s="47"/>
+      <c r="Q39" s="47"/>
+      <c r="R39" s="47"/>
+      <c r="S39" s="47"/>
+      <c r="T39" s="47"/>
       <c r="V39" s="19"/>
     </row>
     <row r="40" spans="1:22" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47" t="s">
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="L40" s="47" t="s">
+      <c r="L40" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47" t="s">
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="46"/>
+      <c r="P40" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="Q40" s="47"/>
-      <c r="R40" s="47"/>
-      <c r="S40" s="47"/>
-      <c r="T40" s="47"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="46"/>
+      <c r="S40" s="46"/>
+      <c r="T40" s="46"/>
       <c r="V40" s="19"/>
     </row>
     <row r="41" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="47" t="s">
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="46"/>
+      <c r="P41" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="Q41" s="47"/>
+      <c r="Q41" s="46"/>
       <c r="R41" s="11" t="s">
         <v>4</v>
       </c>
@@ -3199,249 +3246,288 @@
       <c r="B42" s="39">
         <v>8</v>
       </c>
-      <c r="C42" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="50"/>
+      <c r="C42" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="45"/>
       <c r="K42" s="39">
         <v>6</v>
       </c>
-      <c r="L42" s="51" t="str">
-        <f>L32</f>
-        <v>Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
-      </c>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="51"/>
-      <c r="P42" s="45" t="e">
+      <c r="L42" s="57" t="str">
+        <f>L30</f>
+        <v>Jesus Gonzalez, Gabriel Flores  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
+      </c>
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="41">
         <f>P32</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="36" t="e">
-        <f>S32 + "12:01:00"</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S42" s="36" t="e">
+        <v>45875</v>
+      </c>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="36">
+        <f>S32</f>
+        <v>0.51388888888888884</v>
+      </c>
+      <c r="S42" s="36">
         <f>R42+T42</f>
-        <v>#REF!</v>
+        <v>0.51666666666666661</v>
       </c>
       <c r="T42" s="40">
         <v>2.7777777777777779E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="4" customFormat="1" ht="82.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" s="4" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="39">
         <v>9</v>
       </c>
-      <c r="C43" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="50"/>
+      <c r="C43" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="45"/>
       <c r="K43" s="39">
         <v>7</v>
       </c>
-      <c r="L43" s="99" t="str">
-        <f>L42</f>
-        <v>Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
-      </c>
-      <c r="M43" s="100"/>
-      <c r="N43" s="100"/>
-      <c r="O43" s="101"/>
-      <c r="P43" s="45" t="e">
+      <c r="L43" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="57"/>
+      <c r="P43" s="41">
         <f>P42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="36" t="e">
-        <f t="shared" ref="R43" si="8">S42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S43" s="36" t="e">
-        <f t="shared" ref="S43" si="9">R43+T43</f>
-        <v>#REF!</v>
+        <v>45875</v>
+      </c>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="36">
+        <f>S42</f>
+        <v>0.51666666666666661</v>
+      </c>
+      <c r="S43" s="36">
+        <f>R43+T43</f>
+        <v>0.51944444444444438</v>
       </c>
       <c r="T43" s="40">
         <v>2.7777777777777779E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="10" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="9"/>
-    </row>
-    <row r="45" spans="1:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
-      <c r="C45" s="96" t="s">
+    <row r="44" spans="1:22" s="4" customFormat="1" ht="82.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="39">
+        <v>10</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="39">
+        <v>8</v>
+      </c>
+      <c r="L44" s="48" t="str">
+        <f>L32</f>
+        <v>Leonardo Vera, Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
+      </c>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="41">
+        <f>P42</f>
+        <v>45875</v>
+      </c>
+      <c r="Q44" s="42"/>
+      <c r="R44" s="36">
+        <f>S43</f>
+        <v>0.51944444444444438</v>
+      </c>
+      <c r="S44" s="36">
+        <f t="shared" ref="S44" si="7">R44+T44</f>
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="T44" s="40">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" s="10" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="9"/>
+    </row>
+    <row r="46" spans="1:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="20"/>
+      <c r="C46" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="97"/>
-      <c r="E45" s="97"/>
-      <c r="F45" s="97"/>
-      <c r="G45" s="98"/>
-      <c r="H45" s="91" t="s">
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="91"/>
-      <c r="M45" s="91"/>
-      <c r="N45" s="91" t="s">
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="O45" s="91"/>
-      <c r="P45" s="91"/>
-      <c r="Q45" s="91"/>
-      <c r="R45" s="91"/>
-      <c r="S45" s="91"/>
-      <c r="T45" s="91"/>
-    </row>
-    <row r="46" spans="1:22" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="21">
+      <c r="O46" s="58"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="58"/>
+      <c r="S46" s="58"/>
+      <c r="T46" s="58"/>
+    </row>
+    <row r="47" spans="1:22" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="21">
         <v>1</v>
       </c>
-      <c r="C46" s="90" t="s">
+      <c r="C47" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="92" t="s">
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
+      <c r="M47" s="61"/>
+      <c r="N47" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="O47" s="62"/>
+      <c r="P47" s="62"/>
+      <c r="Q47" s="62"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="62"/>
+      <c r="T47" s="62"/>
+    </row>
+    <row r="48" spans="1:22" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="21">
+        <v>2</v>
+      </c>
+      <c r="C48" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="I46" s="93"/>
-      <c r="J46" s="93"/>
-      <c r="K46" s="93"/>
-      <c r="L46" s="93"/>
-      <c r="M46" s="94"/>
-      <c r="N46" s="95" t="s">
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="60"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="O46" s="95"/>
-      <c r="P46" s="95"/>
-      <c r="Q46" s="95"/>
-      <c r="R46" s="95"/>
-      <c r="S46" s="95"/>
-      <c r="T46" s="95"/>
-    </row>
-    <row r="47" spans="1:22" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="21">
-        <v>2</v>
-      </c>
-      <c r="C47" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="92" t="s">
-        <v>115</v>
-      </c>
-      <c r="I47" s="93"/>
-      <c r="J47" s="93"/>
-      <c r="K47" s="93"/>
-      <c r="L47" s="93"/>
-      <c r="M47" s="94"/>
-      <c r="N47" s="95" t="s">
+      <c r="O48" s="62"/>
+      <c r="P48" s="62"/>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="62"/>
+      <c r="T48" s="62"/>
+      <c r="U48" s="1"/>
+    </row>
+    <row r="49" spans="1:21" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="26">
+        <v>3</v>
+      </c>
+      <c r="C49" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="O47" s="95"/>
-      <c r="P47" s="95"/>
-      <c r="Q47" s="95"/>
-      <c r="R47" s="95"/>
-      <c r="S47" s="95"/>
-      <c r="T47" s="95"/>
-      <c r="U47" s="1"/>
-    </row>
-    <row r="48" spans="1:22" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="26">
-        <v>3</v>
-      </c>
-      <c r="C48" s="83" t="s">
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="I49" s="67"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="67"/>
+      <c r="M49" s="68"/>
+      <c r="N49" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="84"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="86" t="s">
-        <v>121</v>
-      </c>
-      <c r="I48" s="87"/>
-      <c r="J48" s="87"/>
-      <c r="K48" s="87"/>
-      <c r="L48" s="87"/>
-      <c r="M48" s="88"/>
-      <c r="N48" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="O48" s="89"/>
-      <c r="P48" s="89"/>
-      <c r="Q48" s="89"/>
-      <c r="R48" s="89"/>
-      <c r="S48" s="89"/>
-      <c r="T48" s="89"/>
-      <c r="U48" s="1"/>
-    </row>
-    <row r="49" spans="1:21" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="9" t="s">
+      <c r="O49" s="69"/>
+      <c r="P49" s="69"/>
+      <c r="Q49" s="69"/>
+      <c r="R49" s="69"/>
+      <c r="S49" s="69"/>
+      <c r="T49" s="69"/>
+      <c r="U49" s="1"/>
+    </row>
+    <row r="50" spans="1:21" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="22"/>
-      <c r="S49" s="22"/>
-      <c r="T49" s="22"/>
-      <c r="U49" s="22"/>
-    </row>
-    <row r="50" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+      <c r="T50" s="22"/>
+      <c r="U50" s="22"/>
+    </row>
     <row r="51" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3450,41 +3536,59 @@
     <row r="56" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
-  <mergeCells count="99">
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="L40:O41"/>
-    <mergeCell ref="B39:T39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P40:T40"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="H45:M45"/>
-    <mergeCell ref="N45:T45"/>
-    <mergeCell ref="H46:M46"/>
-    <mergeCell ref="H47:M47"/>
-    <mergeCell ref="N46:T46"/>
-    <mergeCell ref="N47:T47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="N48:T48"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
+  <mergeCells count="102">
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:T38"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:T36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:T37"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="B35:T35"/>
+    <mergeCell ref="B34:T34"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="B27:T27"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="B20:T20"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B22:T22"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="C23:J24"/>
+    <mergeCell ref="B21:T21"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="L23:O24"/>
+    <mergeCell ref="E11:T11"/>
+    <mergeCell ref="E18:T18"/>
+    <mergeCell ref="E14:T14"/>
+    <mergeCell ref="E15:T15"/>
+    <mergeCell ref="E16:T16"/>
+    <mergeCell ref="E17:T17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E12:T12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E10:T10"/>
+    <mergeCell ref="G1:P5"/>
+    <mergeCell ref="B1:F6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="P9:T9"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:T19"/>
     <mergeCell ref="B11:D11"/>
@@ -3501,57 +3605,43 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E10:T10"/>
-    <mergeCell ref="G1:P5"/>
-    <mergeCell ref="B1:F6"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E12:T12"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E11:T11"/>
-    <mergeCell ref="E18:T18"/>
-    <mergeCell ref="E14:T14"/>
-    <mergeCell ref="E15:T15"/>
-    <mergeCell ref="E16:T16"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="P9:T9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="E17:T17"/>
-    <mergeCell ref="B20:T20"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B22:T22"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="C23:J24"/>
-    <mergeCell ref="B21:T21"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="L23:O24"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="H49:M49"/>
+    <mergeCell ref="N49:T49"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="H46:M46"/>
+    <mergeCell ref="N46:T46"/>
+    <mergeCell ref="H47:M47"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="N47:T47"/>
+    <mergeCell ref="N48:T48"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P40:T40"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="L40:O41"/>
+    <mergeCell ref="B39:T39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="L44:O44"/>
     <mergeCell ref="C43:J43"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="B35:T35"/>
-    <mergeCell ref="B34:T34"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:T38"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:T36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:T37"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="B27:T27"/>
     <mergeCell ref="L43:O43"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="C40:J41"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="P43:Q43"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3646,7 +3736,7 @@
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:A1048576"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3656,122 +3746,122 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -4091,6 +4181,73 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">76YR7MNCUE67-1366-231</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">
+      <Url>http://bnopsppcwb01-a/grupos-trabajo/ComputoCentral/Oper/_layouts/15/DocIdRedir.aspx?ID=76YR7MNCUE67-1366-231</Url>
+      <Description>76YR7MNCUE67-1366-231</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5050E1606FC674C9C686790EB50E967" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c036e7aa0ed072b5249f02141800f6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d91414de07c556464f3efce90b4366e" ns2:_="">
     <xsd:import namespace="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01"/>
@@ -4235,74 +4392,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A057CF1-CE20-472D-8ADC-CC0274EDD736}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">76YR7MNCUE67-1366-231</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">
-      <Url>http://bnopsppcwb01-a/grupos-trabajo/ComputoCentral/Oper/_layouts/15/DocIdRedir.aspx?ID=76YR7MNCUE67-1366-231</Url>
-      <Description>76YR7MNCUE67-1366-231</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9137EF8C-429C-4D90-951E-D62C9A7F42CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{182B804B-09AD-4BD4-A1A0-384A5F23E9AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C53D4E0-45A7-40DE-B21B-6170E33D1732}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4318,36 +4440,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{182B804B-09AD-4BD4-A1A0-384A5F23E9AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9137EF8C-429C-4D90-951E-D62C9A7F42CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A057CF1-CE20-472D-8ADC-CC0274EDD736}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificacion de numeracion de pasos a ejecutar
</commit_message>
<xml_diff>
--- a/cambios/RFCXXXX/Plan de liberaciones v9.0 RFC----..xlsx
+++ b/cambios/RFCXXXX/Plan de liberaciones v9.0 RFC----..xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\githubppm\PPM\cambios\RFCXXXX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55AB9A5-B19C-4257-9FFB-15AC1C0EB4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E6332-6D79-4858-963E-AA3012824C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1386,6 +1386,189 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1398,12 +1581,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1414,183 +1591,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2019,8 +2019,8 @@
   </sheetPr>
   <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,145 +2050,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="78" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="73" t="s">
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="73"/>
-      <c r="S1" s="74" t="s">
+      <c r="R1" s="66"/>
+      <c r="S1" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="74"/>
+      <c r="T1" s="67"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
     </row>
     <row r="4" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="79" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="R4" s="80"/>
-      <c r="S4" s="83">
+      <c r="R4" s="72"/>
+      <c r="S4" s="75">
         <v>45866</v>
       </c>
-      <c r="T4" s="84"/>
+      <c r="T4" s="76"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="86"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="77"/>
+      <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="75" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="78" t="s">
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
       <c r="U6" s="5"/>
     </row>
     <row r="7" spans="1:21" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2215,457 +2215,457 @@
     </row>
     <row r="8" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
       <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="87" t="s">
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="87"/>
+      <c r="F9" s="79"/>
       <c r="G9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="89" t="s">
+      <c r="H9" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="90"/>
-      <c r="J9" s="91" t="s">
+      <c r="I9" s="57"/>
+      <c r="J9" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="92"/>
-      <c r="L9" s="96" t="s">
+      <c r="K9" s="59"/>
+      <c r="L9" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="97"/>
-      <c r="N9" s="98"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="65"/>
       <c r="O9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="P9" s="93" t="s">
+      <c r="P9" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="94"/>
-      <c r="T9" s="95"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="62"/>
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="72" t="s">
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="72"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="72"/>
-      <c r="Q11" s="72"/>
-      <c r="R11" s="72"/>
-      <c r="S11" s="72"/>
-      <c r="T11" s="72"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
-      <c r="R12" s="72"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="72"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
       <c r="U12" s="5"/>
     </row>
     <row r="13" spans="1:21" ht="88.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="72" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="72"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="72"/>
-      <c r="T13" s="72"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="72" t="s">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="72"/>
-      <c r="S14" s="72"/>
-      <c r="T14" s="72"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="72" t="s">
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="72"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="72" t="s">
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="72"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="72" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="72"/>
-      <c r="S17" s="72"/>
-      <c r="T17" s="72"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="72" t="s">
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="72"/>
-      <c r="Q18" s="72"/>
-      <c r="R18" s="72"/>
-      <c r="S18" s="72"/>
-      <c r="T18" s="72"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="47"/>
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:22" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="72" t="s">
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="72"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
       <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:22" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99"/>
-      <c r="M20" s="99"/>
-      <c r="N20" s="99"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="99"/>
-      <c r="Q20" s="99"/>
-      <c r="R20" s="99"/>
-      <c r="S20" s="99"/>
-      <c r="T20" s="99"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53"/>
+      <c r="T20" s="53"/>
     </row>
     <row r="21" spans="1:22" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
       <c r="U21" s="9"/>
     </row>
     <row r="22" spans="1:22" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="47"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
       <c r="U22" s="9"/>
     </row>
     <row r="23" spans="1:22" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46" t="s">
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46" t="s">
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
     </row>
     <row r="24" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="Q24" s="46"/>
+      <c r="Q24" s="43"/>
       <c r="R24" s="11" t="s">
         <v>4</v>
       </c>
@@ -2681,25 +2681,25 @@
       <c r="B25" s="13">
         <v>1</v>
       </c>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="100"/>
-      <c r="H25" s="100"/>
-      <c r="I25" s="100"/>
-      <c r="J25" s="100"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
       <c r="K25" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="57" t="s">
+      <c r="L25" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
       <c r="P25" s="41">
         <v>45875</v>
       </c>
@@ -2722,26 +2722,26 @@
       <c r="B26" s="13">
         <v>2</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="56"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="52"/>
       <c r="K26" s="13">
         <v>1</v>
       </c>
-      <c r="L26" s="57" t="str">
+      <c r="L26" s="44" t="str">
         <f>L25</f>
         <v>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</v>
       </c>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
       <c r="P26" s="41">
         <f t="shared" ref="P26" si="0">P25</f>
         <v>45875</v>
@@ -2763,27 +2763,27 @@
     </row>
     <row r="27" spans="1:22" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="47"/>
-      <c r="R27" s="47"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="48"/>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
       <c r="U27" s="9"/>
     </row>
     <row r="28" spans="1:22" s="9" customFormat="1" ht="98.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -2791,26 +2791,26 @@
       <c r="B28" s="13">
         <v>3</v>
       </c>
-      <c r="C28" s="100" t="s">
+      <c r="C28" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="100"/>
-      <c r="J28" s="100"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
       <c r="K28" s="13">
         <v>2</v>
       </c>
-      <c r="L28" s="57" t="str">
+      <c r="L28" s="44" t="str">
         <f>L26</f>
         <v>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</v>
       </c>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
       <c r="P28" s="41">
         <f>P26</f>
         <v>45875</v>
@@ -2834,26 +2834,26 @@
       <c r="B29" s="13">
         <v>4</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="56"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="52"/>
       <c r="K29" s="13">
         <v>3</v>
       </c>
-      <c r="L29" s="57" t="str">
+      <c r="L29" s="44" t="str">
         <f>L28</f>
         <v>José Vladimir Herrera Sánchez / Subgerencia de Infraestructura de TI</v>
       </c>
-      <c r="M29" s="57"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="57"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
       <c r="P29" s="41">
         <f>P28</f>
         <v>45875</v>
@@ -2878,25 +2878,25 @@
       <c r="B30" s="13">
         <v>5</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="56"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="52"/>
       <c r="K30" s="13">
         <v>4</v>
       </c>
-      <c r="L30" s="57" t="s">
+      <c r="L30" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="57"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
       <c r="P30" s="41">
         <f>P28</f>
         <v>45875</v>
@@ -2921,25 +2921,25 @@
       <c r="B31" s="35">
         <v>6</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="56"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="52"/>
       <c r="K31" s="35">
-        <v>4</v>
-      </c>
-      <c r="L31" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="L31" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
       <c r="P31" s="41">
         <f>P30</f>
         <v>45875</v>
@@ -2964,26 +2964,26 @@
       <c r="B32" s="13">
         <v>7</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="56"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="52"/>
       <c r="K32" s="13">
-        <v>5</v>
-      </c>
-      <c r="L32" s="57" t="str">
+        <v>6</v>
+      </c>
+      <c r="L32" s="44" t="str">
         <f>L31</f>
         <v>Leonardo Vera, Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
       </c>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
       <c r="P32" s="41">
         <f>P30</f>
         <v>45875</v>
@@ -3029,208 +3029,208 @@
     </row>
     <row r="34" spans="1:22" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
-      <c r="B34" s="101" t="s">
+      <c r="B34" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="101"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
-      <c r="O34" s="101"/>
-      <c r="P34" s="101"/>
-      <c r="Q34" s="101"/>
-      <c r="R34" s="101"/>
-      <c r="S34" s="101"/>
-      <c r="T34" s="101"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
       <c r="U34" s="17"/>
     </row>
     <row r="35" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="47"/>
-      <c r="Q35" s="47"/>
-      <c r="R35" s="47"/>
-      <c r="S35" s="47"/>
-      <c r="T35" s="47"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="48"/>
+      <c r="P35" s="48"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="48"/>
+      <c r="T35" s="48"/>
     </row>
     <row r="36" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="71" t="s">
+      <c r="B36" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="72" t="s">
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="72"/>
-      <c r="M36" s="72"/>
-      <c r="N36" s="72"/>
-      <c r="O36" s="72"/>
-      <c r="P36" s="72"/>
-      <c r="Q36" s="72"/>
-      <c r="R36" s="72"/>
-      <c r="S36" s="72"/>
-      <c r="T36" s="72"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
       <c r="U36" s="5"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="72" t="s">
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
-      <c r="O37" s="72"/>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="47"/>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="47"/>
+      <c r="R37" s="47"/>
+      <c r="S37" s="47"/>
+      <c r="T37" s="47"/>
       <c r="U37" s="5"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="71" t="s">
+      <c r="B38" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="72" t="s">
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="72"/>
-      <c r="N38" s="72"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="72"/>
-      <c r="Q38" s="72"/>
-      <c r="R38" s="72"/>
-      <c r="S38" s="72"/>
-      <c r="T38" s="72"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="47"/>
+      <c r="R38" s="47"/>
+      <c r="S38" s="47"/>
+      <c r="T38" s="47"/>
       <c r="U38" s="5"/>
     </row>
     <row r="39" spans="1:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="47"/>
-      <c r="O39" s="47"/>
-      <c r="P39" s="47"/>
-      <c r="Q39" s="47"/>
-      <c r="R39" s="47"/>
-      <c r="S39" s="47"/>
-      <c r="T39" s="47"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="48"/>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="48"/>
+      <c r="T39" s="48"/>
       <c r="V39" s="19"/>
     </row>
     <row r="40" spans="1:22" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="46" t="s">
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="L40" s="46" t="s">
+      <c r="L40" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="46"/>
-      <c r="P40" s="46" t="s">
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="Q40" s="46"/>
-      <c r="R40" s="46"/>
-      <c r="S40" s="46"/>
-      <c r="T40" s="46"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="43"/>
+      <c r="T40" s="43"/>
       <c r="V40" s="19"/>
     </row>
     <row r="41" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="46"/>
-      <c r="N41" s="46"/>
-      <c r="O41" s="46"/>
-      <c r="P41" s="46" t="s">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="Q41" s="46"/>
+      <c r="Q41" s="43"/>
       <c r="R41" s="11" t="s">
         <v>4</v>
       </c>
@@ -3246,26 +3246,26 @@
       <c r="B42" s="39">
         <v>8</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="96" t="s">
         <v>154</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="45"/>
+      <c r="D42" s="97"/>
+      <c r="E42" s="97"/>
+      <c r="F42" s="97"/>
+      <c r="G42" s="97"/>
+      <c r="H42" s="97"/>
+      <c r="I42" s="97"/>
+      <c r="J42" s="98"/>
       <c r="K42" s="39">
-        <v>6</v>
-      </c>
-      <c r="L42" s="57" t="str">
+        <v>7</v>
+      </c>
+      <c r="L42" s="44" t="str">
         <f>L30</f>
         <v>Jesus Gonzalez, Gabriel Flores  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
       </c>
-      <c r="M42" s="57"/>
-      <c r="N42" s="57"/>
-      <c r="O42" s="57"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
       <c r="P42" s="41">
         <f>P32</f>
         <v>45875</v>
@@ -3287,25 +3287,25 @@
       <c r="B43" s="39">
         <v>9</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="45"/>
+      <c r="D43" s="97"/>
+      <c r="E43" s="97"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="97"/>
+      <c r="H43" s="97"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="98"/>
       <c r="K43" s="39">
-        <v>7</v>
-      </c>
-      <c r="L43" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="L43" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="M43" s="57"/>
-      <c r="N43" s="57"/>
-      <c r="O43" s="57"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
       <c r="P43" s="41">
         <f>P42</f>
         <v>45875</v>
@@ -3327,26 +3327,26 @@
       <c r="B44" s="39">
         <v>10</v>
       </c>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="45"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="98"/>
       <c r="K44" s="39">
-        <v>8</v>
-      </c>
-      <c r="L44" s="48" t="str">
+        <v>9</v>
+      </c>
+      <c r="L44" s="99" t="str">
         <f>L32</f>
         <v>Leonardo Vera, Ramiro Avendaño Castellanos, Valeria Velasco Rivera  / Gerencia Ejecutiva de Información de Proyectos y Sostenibilidad</v>
       </c>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="50"/>
+      <c r="M44" s="100"/>
+      <c r="N44" s="100"/>
+      <c r="O44" s="101"/>
       <c r="P44" s="41">
         <f>P42</f>
         <v>45875</v>
@@ -3389,118 +3389,118 @@
     </row>
     <row r="46" spans="1:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="20"/>
-      <c r="C46" s="51" t="s">
+      <c r="C46" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="58" t="s">
+      <c r="D46" s="94"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="94"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58" t="s">
+      <c r="I46" s="88"/>
+      <c r="J46" s="88"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="88"/>
+      <c r="N46" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="O46" s="58"/>
-      <c r="P46" s="58"/>
-      <c r="Q46" s="58"/>
-      <c r="R46" s="58"/>
-      <c r="S46" s="58"/>
-      <c r="T46" s="58"/>
+      <c r="O46" s="88"/>
+      <c r="P46" s="88"/>
+      <c r="Q46" s="88"/>
+      <c r="R46" s="88"/>
+      <c r="S46" s="88"/>
+      <c r="T46" s="88"/>
     </row>
     <row r="47" spans="1:22" s="4" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21">
         <v>1</v>
       </c>
-      <c r="C47" s="70" t="s">
+      <c r="C47" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="59" t="s">
+      <c r="D47" s="87"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="87"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="61"/>
-      <c r="N47" s="62" t="s">
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
+      <c r="M47" s="91"/>
+      <c r="N47" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="O47" s="62"/>
-      <c r="P47" s="62"/>
-      <c r="Q47" s="62"/>
-      <c r="R47" s="62"/>
-      <c r="S47" s="62"/>
-      <c r="T47" s="62"/>
+      <c r="O47" s="92"/>
+      <c r="P47" s="92"/>
+      <c r="Q47" s="92"/>
+      <c r="R47" s="92"/>
+      <c r="S47" s="92"/>
+      <c r="T47" s="92"/>
     </row>
     <row r="48" spans="1:22" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="21">
         <v>2</v>
       </c>
-      <c r="C48" s="70" t="s">
+      <c r="C48" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
-      <c r="H48" s="59" t="s">
+      <c r="D48" s="87"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="87"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="89" t="s">
         <v>114</v>
       </c>
-      <c r="I48" s="60"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="60"/>
-      <c r="L48" s="60"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="62" t="s">
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
+      <c r="M48" s="91"/>
+      <c r="N48" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="O48" s="62"/>
-      <c r="P48" s="62"/>
-      <c r="Q48" s="62"/>
-      <c r="R48" s="62"/>
-      <c r="S48" s="62"/>
-      <c r="T48" s="62"/>
+      <c r="O48" s="92"/>
+      <c r="P48" s="92"/>
+      <c r="Q48" s="92"/>
+      <c r="R48" s="92"/>
+      <c r="S48" s="92"/>
+      <c r="T48" s="92"/>
       <c r="U48" s="1"/>
     </row>
     <row r="49" spans="1:21" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="26">
         <v>3</v>
       </c>
-      <c r="C49" s="63" t="s">
+      <c r="C49" s="80" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="66" t="s">
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="I49" s="67"/>
-      <c r="J49" s="67"/>
-      <c r="K49" s="67"/>
-      <c r="L49" s="67"/>
-      <c r="M49" s="68"/>
-      <c r="N49" s="69" t="s">
+      <c r="I49" s="84"/>
+      <c r="J49" s="84"/>
+      <c r="K49" s="84"/>
+      <c r="L49" s="84"/>
+      <c r="M49" s="85"/>
+      <c r="N49" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="O49" s="69"/>
-      <c r="P49" s="69"/>
-      <c r="Q49" s="69"/>
-      <c r="R49" s="69"/>
-      <c r="S49" s="69"/>
-      <c r="T49" s="69"/>
+      <c r="O49" s="86"/>
+      <c r="P49" s="86"/>
+      <c r="Q49" s="86"/>
+      <c r="R49" s="86"/>
+      <c r="S49" s="86"/>
+      <c r="T49" s="86"/>
       <c r="U49" s="1"/>
     </row>
     <row r="50" spans="1:21" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3540,47 +3540,40 @@
   </sheetData>
   <sheetProtection formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="102">
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="C40:J41"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:T38"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:T36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:T37"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="B35:T35"/>
-    <mergeCell ref="B34:T34"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="B27:T27"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="B20:T20"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B22:T22"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="C23:J24"/>
-    <mergeCell ref="B21:T21"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="L23:O24"/>
-    <mergeCell ref="E11:T11"/>
-    <mergeCell ref="E18:T18"/>
-    <mergeCell ref="E14:T14"/>
-    <mergeCell ref="E15:T15"/>
-    <mergeCell ref="E16:T16"/>
-    <mergeCell ref="E17:T17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E12:T12"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="L40:O41"/>
+    <mergeCell ref="B39:T39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="L43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P40:T40"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="H49:M49"/>
+    <mergeCell ref="N49:T49"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="H46:M46"/>
+    <mergeCell ref="N46:T46"/>
+    <mergeCell ref="H47:M47"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="N47:T47"/>
+    <mergeCell ref="N48:T48"/>
+    <mergeCell ref="C46:G46"/>
     <mergeCell ref="E10:T10"/>
     <mergeCell ref="G1:P5"/>
     <mergeCell ref="B1:F6"/>
@@ -3605,43 +3598,50 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="H49:M49"/>
-    <mergeCell ref="N49:T49"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="H46:M46"/>
-    <mergeCell ref="N46:T46"/>
-    <mergeCell ref="H47:M47"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="N47:T47"/>
-    <mergeCell ref="N48:T48"/>
-    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="E11:T11"/>
+    <mergeCell ref="E18:T18"/>
+    <mergeCell ref="E14:T14"/>
+    <mergeCell ref="E15:T15"/>
+    <mergeCell ref="E16:T16"/>
+    <mergeCell ref="E17:T17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E12:T12"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B20:T20"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B22:T22"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="C23:J24"/>
+    <mergeCell ref="B21:T21"/>
+    <mergeCell ref="P23:T23"/>
+    <mergeCell ref="L23:O24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="C40:J41"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:T38"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:T36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:T37"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="B35:T35"/>
+    <mergeCell ref="B34:T34"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="B27:T27"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
     <mergeCell ref="C31:J31"/>
     <mergeCell ref="L31:O31"/>
     <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P40:T40"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="L40:O41"/>
-    <mergeCell ref="B39:T39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="L43:O43"/>
-    <mergeCell ref="P43:Q43"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3735,7 +3735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EFD11B3-151E-4452-B8FD-33EA45A24AC8}">
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -4181,73 +4181,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">76YR7MNCUE67-1366-231</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">
-      <Url>http://bnopsppcwb01-a/grupos-trabajo/ComputoCentral/Oper/_layouts/15/DocIdRedir.aspx?ID=76YR7MNCUE67-1366-231</Url>
-      <Description>76YR7MNCUE67-1366-231</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5050E1606FC674C9C686790EB50E967" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c036e7aa0ed072b5249f02141800f6be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d91414de07c556464f3efce90b4366e" ns2:_="">
     <xsd:import namespace="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01"/>
@@ -4392,15 +4325,100 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">76YR7MNCUE67-1366-231</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01">
+      <Url>http://bnopsppcwb01-a/grupos-trabajo/ComputoCentral/Oper/_layouts/15/DocIdRedir.aspx?ID=76YR7MNCUE67-1366-231</Url>
+      <Description>76YR7MNCUE67-1366-231</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A057CF1-CE20-472D-8ADC-CC0274EDD736}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C53D4E0-45A7-40DE-B21B-6170E33D1732}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{182B804B-09AD-4BD4-A1A0-384A5F23E9AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9137EF8C-429C-4D90-951E-D62C9A7F42CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -4416,28 +4434,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{182B804B-09AD-4BD4-A1A0-384A5F23E9AC}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A057CF1-CE20-472D-8ADC-CC0274EDD736}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C53D4E0-45A7-40DE-B21B-6170E33D1732}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a22a6dd2-ec3f-4630-af3d-38cc2a3baf01"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Extension de horario de validaciones
</commit_message>
<xml_diff>
--- a/cambios/RFCXXXX/Plan de liberaciones v9.0 RFC----..xlsx
+++ b/cambios/RFCXXXX/Plan de liberaciones v9.0 RFC----..xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\githubppm\PPM\cambios\RFCXXXX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E6332-6D79-4858-963E-AA3012824C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E3FCDF-7898-4E95-B44B-6EC31749A2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2019,8 +2019,8 @@
   </sheetPr>
   <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W44" sqref="W44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,11 +2950,11 @@
         <v>0.47222222222222221</v>
       </c>
       <c r="S31" s="36">
-        <f t="shared" ref="S31" si="5">R31+T31</f>
-        <v>0.5</v>
+        <f>R31+T31</f>
+        <v>0.52083333333333337</v>
       </c>
       <c r="T31" s="40">
-        <v>2.7777777777777776E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="U31" s="37"/>
       <c r="V31" s="38"/>
@@ -2991,14 +2991,14 @@
       <c r="Q32" s="42"/>
       <c r="R32" s="14">
         <f>S31</f>
-        <v>0.5</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="S32" s="14">
-        <f t="shared" ref="S32" si="6">R32+T32</f>
-        <v>0.51388888888888884</v>
+        <f>R32+T32</f>
+        <v>0.54166666666666674</v>
       </c>
       <c r="T32" s="25">
-        <v>1.3888888888888888E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="U32" s="15"/>
       <c r="V32" s="16"/>
@@ -3273,11 +3273,11 @@
       <c r="Q42" s="42"/>
       <c r="R42" s="36">
         <f>S32</f>
-        <v>0.51388888888888884</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="S42" s="36">
         <f>R42+T42</f>
-        <v>0.51666666666666661</v>
+        <v>0.54444444444444451</v>
       </c>
       <c r="T42" s="40">
         <v>2.7777777777777779E-3</v>
@@ -3313,11 +3313,11 @@
       <c r="Q43" s="42"/>
       <c r="R43" s="36">
         <f>S42</f>
-        <v>0.51666666666666661</v>
+        <v>0.54444444444444451</v>
       </c>
       <c r="S43" s="36">
         <f>R43+T43</f>
-        <v>0.51944444444444438</v>
+        <v>0.54722222222222228</v>
       </c>
       <c r="T43" s="40">
         <v>2.7777777777777779E-3</v>
@@ -3354,11 +3354,11 @@
       <c r="Q44" s="42"/>
       <c r="R44" s="36">
         <f>S43</f>
-        <v>0.51944444444444438</v>
+        <v>0.54722222222222228</v>
       </c>
       <c r="S44" s="36">
-        <f t="shared" ref="S44" si="7">R44+T44</f>
-        <v>0.54722222222222217</v>
+        <f t="shared" ref="S44" si="5">R44+T44</f>
+        <v>0.57500000000000007</v>
       </c>
       <c r="T44" s="40">
         <v>2.7777777777777776E-2</v>

</xml_diff>